<commit_message>
Model updated and folder re-structure
</commit_message>
<xml_diff>
--- a/data/statistics (pacing).xlsx
+++ b/data/statistics (pacing).xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x15 xr xr6 xr10">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24026"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10711"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ezra\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/eashan22/Desktop/Internship 2021/bbrv2/kibana-data-retrieval/src/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:40009_{4B48FAEB-A33A-421E-8405-0FF8951FECA5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{132A862D-D3DC-2241-93CD-C6E17D086B0B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2025" yWindow="1710" windowWidth="47085" windowHeight="29745"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="33600" windowHeight="19340" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="statistics (pacing)" sheetId="1" r:id="rId1"/>
@@ -565,7 +565,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="18" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -5676,21 +5676,30 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AG75"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="AK89" sqref="AK89"/>
+    <sheetView tabSelected="1" zoomScale="75" workbookViewId="0">
+      <selection activeCell="J1" sqref="J1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="5" max="5" width="23.5703125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="21.7109375" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="23.140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="23.5" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="9" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="21.83203125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="23.33203125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="12.5" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="12.6640625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="13.1640625" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="11.5" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="17.6640625" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="12.1640625" bestFit="1" customWidth="1"/>
+    <col min="22" max="25" width="11.1640625" bestFit="1" customWidth="1"/>
+    <col min="30" max="31" width="11.1640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:33" x14ac:dyDescent="0.2">
       <c r="B1" t="s">
         <v>0</v>
       </c>
@@ -5767,7 +5776,7 @@
         <v>178</v>
       </c>
     </row>
-    <row r="2" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:33" x14ac:dyDescent="0.2">
       <c r="A2">
         <v>0</v>
       </c>
@@ -5847,7 +5856,7 @@
         <v>972525407.03930998</v>
       </c>
     </row>
-    <row r="3" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:33" x14ac:dyDescent="0.2">
       <c r="A3">
         <v>1</v>
       </c>
@@ -5927,7 +5936,7 @@
         <v>1941758307.586</v>
       </c>
     </row>
-    <row r="4" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:33" x14ac:dyDescent="0.2">
       <c r="A4">
         <v>2</v>
       </c>
@@ -6007,7 +6016,7 @@
         <v>2569156003.6378598</v>
       </c>
     </row>
-    <row r="5" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:33" x14ac:dyDescent="0.2">
       <c r="A5">
         <v>3</v>
       </c>
@@ -6087,7 +6096,7 @@
         <v>2891742310.5822301</v>
       </c>
     </row>
-    <row r="6" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:33" x14ac:dyDescent="0.2">
       <c r="A6">
         <v>4</v>
       </c>
@@ -6167,7 +6176,7 @@
         <v>2680629628.8148198</v>
       </c>
     </row>
-    <row r="7" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:33" x14ac:dyDescent="0.2">
       <c r="A7">
         <v>5</v>
       </c>
@@ -6247,7 +6256,7 @@
         <v>2051859918.76109</v>
       </c>
     </row>
-    <row r="8" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:33" x14ac:dyDescent="0.2">
       <c r="A8">
         <v>6</v>
       </c>
@@ -6297,7 +6306,7 @@
         <v>36803996368</v>
       </c>
     </row>
-    <row r="9" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:33" x14ac:dyDescent="0.2">
       <c r="A9">
         <v>7</v>
       </c>
@@ -6347,7 +6356,7 @@
         <v>44157328052</v>
       </c>
     </row>
-    <row r="10" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:33" x14ac:dyDescent="0.2">
       <c r="A10">
         <v>20</v>
       </c>
@@ -6397,7 +6406,7 @@
         <v>7388940684</v>
       </c>
     </row>
-    <row r="11" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:33" x14ac:dyDescent="0.2">
       <c r="A11">
         <v>21</v>
       </c>
@@ -6462,7 +6471,7 @@
         <v>178</v>
       </c>
     </row>
-    <row r="12" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:33" x14ac:dyDescent="0.2">
       <c r="A12">
         <v>22</v>
       </c>
@@ -6527,7 +6536,7 @@
         <v>5477012689.6185198</v>
       </c>
     </row>
-    <row r="13" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:33" x14ac:dyDescent="0.2">
       <c r="A13">
         <v>23</v>
       </c>
@@ -6592,7 +6601,7 @@
         <v>1908713042.7536199</v>
       </c>
     </row>
-    <row r="14" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:33" x14ac:dyDescent="0.2">
       <c r="A14">
         <v>24</v>
       </c>
@@ -6657,7 +6666,7 @@
         <v>2468477098.5858698</v>
       </c>
     </row>
-    <row r="15" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:33" x14ac:dyDescent="0.2">
       <c r="A15">
         <v>25</v>
       </c>
@@ -6722,7 +6731,7 @@
         <v>2608295127.6458402</v>
       </c>
     </row>
-    <row r="16" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:33" x14ac:dyDescent="0.2">
       <c r="A16">
         <v>38</v>
       </c>
@@ -6787,7 +6796,7 @@
         <v>3014614923.3134398</v>
       </c>
     </row>
-    <row r="17" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A17">
         <v>39</v>
       </c>
@@ -6852,7 +6861,7 @@
         <v>2308398445.27039</v>
       </c>
     </row>
-    <row r="18" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A18">
         <v>40</v>
       </c>
@@ -6902,7 +6911,7 @@
         <v>21606140496</v>
       </c>
     </row>
-    <row r="19" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A19">
         <v>41</v>
       </c>
@@ -6952,7 +6961,7 @@
         <v>28784485588</v>
       </c>
     </row>
-    <row r="20" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A20">
         <v>42</v>
       </c>
@@ -7002,7 +7011,7 @@
         <v>35948129116</v>
       </c>
     </row>
-    <row r="21" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A21">
         <v>43</v>
       </c>
@@ -7052,7 +7061,7 @@
         <v>43138205036</v>
       </c>
     </row>
-    <row r="22" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A22">
         <v>56</v>
       </c>
@@ -7102,7 +7111,7 @@
         <v>7217819132</v>
       </c>
     </row>
-    <row r="23" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A23">
         <v>57</v>
       </c>
@@ -7152,7 +7161,7 @@
         <v>14466951852</v>
       </c>
     </row>
-    <row r="24" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A24">
         <v>58</v>
       </c>
@@ -7202,7 +7211,7 @@
         <v>17534612588</v>
       </c>
     </row>
-    <row r="25" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A25">
         <v>59</v>
       </c>
@@ -7252,7 +7261,7 @@
         <v>19309895788</v>
       </c>
     </row>
-    <row r="26" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A26">
         <v>60</v>
       </c>
@@ -7302,7 +7311,7 @@
         <v>18140231124</v>
       </c>
     </row>
-    <row r="27" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A27">
         <v>61</v>
       </c>
@@ -7352,7 +7361,7 @@
         <v>16836400148</v>
       </c>
     </row>
-    <row r="28" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A28">
         <v>8</v>
       </c>
@@ -7402,7 +7411,7 @@
         <v>1822568844</v>
       </c>
     </row>
-    <row r="29" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A29">
         <v>9</v>
       </c>
@@ -7452,7 +7461,7 @@
         <v>1496387400</v>
       </c>
     </row>
-    <row r="30" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A30">
         <v>10</v>
       </c>
@@ -7502,7 +7511,7 @@
         <v>1691024296</v>
       </c>
     </row>
-    <row r="31" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A31">
         <v>11</v>
       </c>
@@ -7552,7 +7561,7 @@
         <v>1624728564</v>
       </c>
     </row>
-    <row r="32" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A32">
         <v>12</v>
       </c>
@@ -7602,7 +7611,7 @@
         <v>1448971948</v>
       </c>
     </row>
-    <row r="33" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A33">
         <v>13</v>
       </c>
@@ -7652,7 +7661,7 @@
         <v>2040005244</v>
       </c>
     </row>
-    <row r="34" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A34">
         <v>26</v>
       </c>
@@ -7702,7 +7711,7 @@
         <v>1884990092</v>
       </c>
     </row>
-    <row r="35" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A35">
         <v>27</v>
       </c>
@@ -7752,7 +7761,7 @@
         <v>2491118664</v>
       </c>
     </row>
-    <row r="36" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A36">
         <v>28</v>
       </c>
@@ -7802,7 +7811,7 @@
         <v>2382982084</v>
       </c>
     </row>
-    <row r="37" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A37">
         <v>29</v>
       </c>
@@ -7852,7 +7861,7 @@
         <v>1678353928</v>
       </c>
     </row>
-    <row r="38" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A38">
         <v>30</v>
       </c>
@@ -7902,7 +7911,7 @@
         <v>2128509912</v>
       </c>
     </row>
-    <row r="39" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A39">
         <v>31</v>
       </c>
@@ -7952,7 +7961,7 @@
         <v>2037714556</v>
       </c>
     </row>
-    <row r="40" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A40">
         <v>44</v>
       </c>
@@ -8002,7 +8011,7 @@
         <v>7151890268</v>
       </c>
     </row>
-    <row r="41" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A41">
         <v>45</v>
       </c>
@@ -8052,7 +8061,7 @@
         <v>14233185352</v>
       </c>
     </row>
-    <row r="42" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A42">
         <v>46</v>
       </c>
@@ -8102,7 +8111,7 @@
         <v>21063596412</v>
       </c>
     </row>
-    <row r="43" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A43">
         <v>47</v>
       </c>
@@ -8152,7 +8161,7 @@
         <v>27585387804</v>
       </c>
     </row>
-    <row r="44" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A44">
         <v>48</v>
       </c>
@@ -8202,7 +8211,7 @@
         <v>34149939036</v>
       </c>
     </row>
-    <row r="45" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A45">
         <v>49</v>
       </c>
@@ -8252,7 +8261,7 @@
         <v>40846747508</v>
       </c>
     </row>
-    <row r="46" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A46">
         <v>62</v>
       </c>
@@ -8302,7 +8311,7 @@
         <v>7153142988</v>
       </c>
     </row>
-    <row r="47" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A47">
         <v>63</v>
       </c>
@@ -8352,7 +8361,7 @@
         <v>14073168268</v>
       </c>
     </row>
-    <row r="48" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A48">
         <v>64</v>
       </c>
@@ -8402,7 +8411,7 @@
         <v>18197435688</v>
       </c>
     </row>
-    <row r="49" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A49">
         <v>65</v>
       </c>
@@ -8452,7 +8461,7 @@
         <v>19278225668</v>
       </c>
     </row>
-    <row r="50" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A50">
         <v>66</v>
       </c>
@@ -8502,7 +8511,7 @@
         <v>22314598396</v>
       </c>
     </row>
-    <row r="51" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A51">
         <v>67</v>
       </c>
@@ -8552,7 +8561,7 @@
         <v>17002958220</v>
       </c>
     </row>
-    <row r="52" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A52">
         <v>14</v>
       </c>
@@ -8602,7 +8611,7 @@
         <v>7410675376</v>
       </c>
     </row>
-    <row r="53" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A53">
         <v>15</v>
       </c>
@@ -8652,7 +8661,7 @@
         <v>14802134984</v>
       </c>
     </row>
-    <row r="54" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A54">
         <v>16</v>
       </c>
@@ -8702,7 +8711,7 @@
         <v>22185219264</v>
       </c>
     </row>
-    <row r="55" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A55">
         <v>17</v>
       </c>
@@ -8752,7 +8761,7 @@
         <v>29576598340</v>
       </c>
     </row>
-    <row r="56" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A56">
         <v>18</v>
       </c>
@@ -8802,7 +8811,7 @@
         <v>36949562432</v>
       </c>
     </row>
-    <row r="57" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A57">
         <v>19</v>
       </c>
@@ -8852,7 +8861,7 @@
         <v>44323964004</v>
       </c>
     </row>
-    <row r="58" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A58">
         <v>32</v>
       </c>
@@ -8902,7 +8911,7 @@
         <v>7409046840</v>
       </c>
     </row>
-    <row r="59" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A59">
         <v>33</v>
       </c>
@@ -8952,7 +8961,7 @@
         <v>14810930868</v>
       </c>
     </row>
-    <row r="60" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A60">
         <v>34</v>
       </c>
@@ -9002,7 +9011,7 @@
         <v>18067689688</v>
       </c>
     </row>
-    <row r="61" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A61">
         <v>35</v>
       </c>
@@ -9052,7 +9061,7 @@
         <v>19630341564</v>
       </c>
     </row>
-    <row r="62" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A62">
         <v>36</v>
       </c>
@@ -9102,7 +9111,7 @@
         <v>19574586576</v>
       </c>
     </row>
-    <row r="63" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A63">
         <v>37</v>
       </c>
@@ -9152,7 +9161,7 @@
         <v>11573213392</v>
       </c>
     </row>
-    <row r="64" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A64">
         <v>50</v>
       </c>
@@ -9202,7 +9211,7 @@
         <v>7240019120</v>
       </c>
     </row>
-    <row r="65" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A65">
         <v>51</v>
       </c>
@@ -9252,7 +9261,7 @@
         <v>14447615224</v>
       </c>
     </row>
-    <row r="66" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A66">
         <v>52</v>
       </c>
@@ -9302,7 +9311,7 @@
         <v>21707995580</v>
       </c>
     </row>
-    <row r="67" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A67">
         <v>53</v>
       </c>
@@ -9352,7 +9361,7 @@
         <v>28910201840</v>
       </c>
     </row>
-    <row r="68" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A68">
         <v>54</v>
       </c>
@@ -9402,7 +9411,7 @@
         <v>36102094204</v>
       </c>
     </row>
-    <row r="69" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A69">
         <v>55</v>
       </c>
@@ -9452,7 +9461,7 @@
         <v>43313031060</v>
       </c>
     </row>
-    <row r="70" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A70">
         <v>68</v>
       </c>
@@ -9502,7 +9511,7 @@
         <v>7243374620</v>
       </c>
     </row>
-    <row r="71" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A71">
         <v>69</v>
       </c>
@@ -9552,7 +9561,7 @@
         <v>14464124284</v>
       </c>
     </row>
-    <row r="72" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A72">
         <v>70</v>
       </c>
@@ -9602,7 +9611,7 @@
         <v>19150591396</v>
       </c>
     </row>
-    <row r="73" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A73">
         <v>71</v>
       </c>
@@ -9652,7 +9661,7 @@
         <v>21544130856</v>
       </c>
     </row>
-    <row r="74" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A74">
         <v>72</v>
       </c>
@@ -9702,7 +9711,7 @@
         <v>19954831836</v>
       </c>
     </row>
-    <row r="75" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A75">
         <v>73</v>
       </c>

</xml_diff>